<commit_message>
run some cell for presentation
</commit_message>
<xml_diff>
--- a/data/processed/test_data_excel.xlsx
+++ b/data/processed/test_data_excel.xlsx
@@ -598,7 +598,7 @@
         <v>3549</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>8</v>
@@ -2715,7 +2715,7 @@
         <v>3227</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" t="n">
         <v>54</v>
@@ -3810,7 +3810,7 @@
         <v>223</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
         <v>10</v>
@@ -4102,7 +4102,7 @@
         <v>134</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" t="n">
         <v>23</v>
@@ -5051,7 +5051,7 @@
         <v>2532</v>
       </c>
       <c r="B64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" t="n">
         <v>37</v>
@@ -5854,7 +5854,7 @@
         <v>4906</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75" t="n">
         <v>26</v>
@@ -6511,7 +6511,7 @@
         <v>414</v>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" t="n">
         <v>17</v>
@@ -6949,7 +6949,7 @@
         <v>1204</v>
       </c>
       <c r="B90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" t="n">
         <v>21</v>
@@ -8117,7 +8117,7 @@
         <v>261</v>
       </c>
       <c r="B106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106" t="n">
         <v>18</v>
@@ -9066,7 +9066,7 @@
         <v>2739</v>
       </c>
       <c r="B119" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C119" t="n">
         <v>13</v>
@@ -10015,7 +10015,7 @@
         <v>1689</v>
       </c>
       <c r="B132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C132" t="n">
         <v>1</v>
@@ -11548,7 +11548,7 @@
         <v>4874</v>
       </c>
       <c r="B153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C153" t="n">
         <v>10</v>
@@ -11621,7 +11621,7 @@
         <v>6457</v>
       </c>
       <c r="B154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C154" t="n">
         <v>72</v>
@@ -12132,7 +12132,7 @@
         <v>656</v>
       </c>
       <c r="B161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C161" t="n">
         <v>36</v>
@@ -12935,7 +12935,7 @@
         <v>5237</v>
       </c>
       <c r="B172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C172" t="n">
         <v>20</v>
@@ -13154,7 +13154,7 @@
         <v>657</v>
       </c>
       <c r="B175" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C175" t="n">
         <v>1</v>
@@ -13227,7 +13227,7 @@
         <v>2015</v>
       </c>
       <c r="B176" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C176" t="n">
         <v>20</v>
@@ -14687,7 +14687,7 @@
         <v>4034</v>
       </c>
       <c r="B196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C196" t="n">
         <v>33</v>
@@ -15709,7 +15709,7 @@
         <v>4359</v>
       </c>
       <c r="B210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C210" t="n">
         <v>1</v>
@@ -16366,7 +16366,7 @@
         <v>5163</v>
       </c>
       <c r="B219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C219" t="n">
         <v>29</v>
@@ -16439,7 +16439,7 @@
         <v>1411</v>
       </c>
       <c r="B220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C220" t="n">
         <v>32</v>
@@ -18702,7 +18702,7 @@
         <v>4868</v>
       </c>
       <c r="B251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C251" t="n">
         <v>55</v>
@@ -21257,7 +21257,7 @@
         <v>5546</v>
       </c>
       <c r="B286" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C286" t="n">
         <v>12</v>
@@ -21695,7 +21695,7 @@
         <v>5425</v>
       </c>
       <c r="B292" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C292" t="n">
         <v>1</v>
@@ -22060,7 +22060,7 @@
         <v>3707</v>
       </c>
       <c r="B297" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C297" t="n">
         <v>28</v>
@@ -24615,7 +24615,7 @@
         <v>4005</v>
       </c>
       <c r="B332" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C332" t="n">
         <v>1</v>
@@ -24688,7 +24688,7 @@
         <v>528</v>
       </c>
       <c r="B333" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C333" t="n">
         <v>49</v>
@@ -28338,7 +28338,7 @@
         <v>6452</v>
       </c>
       <c r="B383" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C383" t="n">
         <v>1</v>
@@ -28703,7 +28703,7 @@
         <v>1677</v>
       </c>
       <c r="B388" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C388" t="n">
         <v>1</v>
@@ -28922,7 +28922,7 @@
         <v>15</v>
       </c>
       <c r="B391" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C391" t="n">
         <v>15</v>
@@ -29141,7 +29141,7 @@
         <v>1878</v>
       </c>
       <c r="B394" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C394" t="n">
         <v>25</v>
@@ -29944,7 +29944,7 @@
         <v>3855</v>
       </c>
       <c r="B405" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C405" t="n">
         <v>7</v>
@@ -30090,7 +30090,7 @@
         <v>3931</v>
       </c>
       <c r="B407" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C407" t="n">
         <v>15</v>
@@ -30455,7 +30455,7 @@
         <v>1482</v>
       </c>
       <c r="B412" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C412" t="n">
         <v>1</v>
@@ -30893,7 +30893,7 @@
         <v>6087</v>
       </c>
       <c r="B418" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C418" t="n">
         <v>1</v>
@@ -31550,7 +31550,7 @@
         <v>2443</v>
       </c>
       <c r="B427" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C427" t="n">
         <v>1</v>
@@ -32061,7 +32061,7 @@
         <v>6360</v>
       </c>
       <c r="B434" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C434" t="n">
         <v>4</v>
@@ -33594,7 +33594,7 @@
         <v>5171</v>
       </c>
       <c r="B455" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C455" t="n">
         <v>3</v>
@@ -38558,7 +38558,7 @@
         <v>5135</v>
       </c>
       <c r="B523" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C523" t="n">
         <v>30</v>
@@ -39288,7 +39288,7 @@
         <v>3087</v>
       </c>
       <c r="B533" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C533" t="n">
         <v>1</v>
@@ -41113,7 +41113,7 @@
         <v>799</v>
       </c>
       <c r="B558" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C558" t="n">
         <v>5</v>
@@ -42500,7 +42500,7 @@
         <v>1471</v>
       </c>
       <c r="B577" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C577" t="n">
         <v>1</v>
@@ -44398,7 +44398,7 @@
         <v>1808</v>
       </c>
       <c r="B603" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C603" t="n">
         <v>13</v>
@@ -45712,7 +45712,7 @@
         <v>1070</v>
       </c>
       <c r="B621" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C621" t="n">
         <v>1</v>
@@ -47026,7 +47026,7 @@
         <v>2438</v>
       </c>
       <c r="B639" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C639" t="n">
         <v>0</v>
@@ -47683,7 +47683,7 @@
         <v>4354</v>
       </c>
       <c r="B648" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C648" t="n">
         <v>46</v>
@@ -47975,7 +47975,7 @@
         <v>1336</v>
       </c>
       <c r="B652" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C652" t="n">
         <v>6</v>
@@ -48559,7 +48559,7 @@
         <v>2189</v>
       </c>
       <c r="B660" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C660" t="n">
         <v>18</v>
@@ -49289,7 +49289,7 @@
         <v>5071</v>
       </c>
       <c r="B670" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C670" t="n">
         <v>5</v>
@@ -51260,7 +51260,7 @@
         <v>220</v>
       </c>
       <c r="B697" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C697" t="n">
         <v>59</v>
@@ -51698,7 +51698,7 @@
         <v>5719</v>
       </c>
       <c r="B703" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C703" t="n">
         <v>0</v>
@@ -52063,7 +52063,7 @@
         <v>6665</v>
       </c>
       <c r="B708" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C708" t="n">
         <v>63</v>
@@ -53742,7 +53742,7 @@
         <v>791</v>
       </c>
       <c r="B731" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C731" t="n">
         <v>50</v>
@@ -54691,7 +54691,7 @@
         <v>4318</v>
       </c>
       <c r="B744" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C744" t="n">
         <v>1</v>
@@ -55713,7 +55713,7 @@
         <v>5021</v>
       </c>
       <c r="B758" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C758" t="n">
         <v>1</v>
@@ -56735,7 +56735,7 @@
         <v>5644</v>
       </c>
       <c r="B772" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C772" t="n">
         <v>5</v>
@@ -57100,7 +57100,7 @@
         <v>5364</v>
       </c>
       <c r="B777" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C777" t="n">
         <v>12</v>
@@ -58706,7 +58706,7 @@
         <v>961</v>
       </c>
       <c r="B799" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C799" t="n">
         <v>1</v>
@@ -60823,7 +60823,7 @@
         <v>29</v>
       </c>
       <c r="B828" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C828" t="n">
         <v>27</v>
@@ -61042,7 +61042,7 @@
         <v>926</v>
       </c>
       <c r="B831" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C831" t="n">
         <v>32</v>
@@ -61407,7 +61407,7 @@
         <v>2066</v>
       </c>
       <c r="B836" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C836" t="n">
         <v>57</v>
@@ -61991,7 +61991,7 @@
         <v>2987</v>
       </c>
       <c r="B844" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C844" t="n">
         <v>56</v>
@@ -62283,7 +62283,7 @@
         <v>4083</v>
       </c>
       <c r="B848" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C848" t="n">
         <v>1</v>
@@ -62940,7 +62940,7 @@
         <v>1967</v>
       </c>
       <c r="B857" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C857" t="n">
         <v>1</v>
@@ -63524,7 +63524,7 @@
         <v>3505</v>
       </c>
       <c r="B865" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C865" t="n">
         <v>38</v>
@@ -65276,7 +65276,7 @@
         <v>4780</v>
       </c>
       <c r="B889" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C889" t="n">
         <v>29</v>
@@ -65495,7 +65495,7 @@
         <v>303</v>
       </c>
       <c r="B892" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C892" t="n">
         <v>60</v>
@@ -66663,7 +66663,7 @@
         <v>2691</v>
       </c>
       <c r="B908" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C908" t="n">
         <v>32</v>
@@ -68196,7 +68196,7 @@
         <v>5838</v>
       </c>
       <c r="B929" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C929" t="n">
         <v>56</v>
@@ -68269,7 +68269,7 @@
         <v>6361</v>
       </c>
       <c r="B930" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C930" t="n">
         <v>1</v>
@@ -69510,7 +69510,7 @@
         <v>4550</v>
       </c>
       <c r="B947" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C947" t="n">
         <v>24</v>
@@ -71408,7 +71408,7 @@
         <v>6033</v>
       </c>
       <c r="B973" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C973" t="n">
         <v>4</v>
@@ -72211,7 +72211,7 @@
         <v>2154</v>
       </c>
       <c r="B984" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C984" t="n">
         <v>48</v>
@@ -73233,7 +73233,7 @@
         <v>1325</v>
       </c>
       <c r="B998" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C998" t="n">
         <v>1</v>
@@ -73890,7 +73890,7 @@
         <v>1169</v>
       </c>
       <c r="B1007" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1007" t="n">
         <v>12</v>
@@ -74401,7 +74401,7 @@
         <v>3950</v>
       </c>
       <c r="B1014" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1014" t="n">
         <v>4</v>
@@ -74912,7 +74912,7 @@
         <v>825</v>
       </c>
       <c r="B1021" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1021" t="n">
         <v>1</v>
@@ -75277,7 +75277,7 @@
         <v>1235</v>
       </c>
       <c r="B1026" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1026" t="n">
         <v>1</v>
@@ -75934,7 +75934,7 @@
         <v>3907</v>
       </c>
       <c r="B1035" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1035" t="n">
         <v>1</v>
@@ -77394,7 +77394,7 @@
         <v>4923</v>
       </c>
       <c r="B1055" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1055" t="n">
         <v>21</v>
@@ -77978,7 +77978,7 @@
         <v>1517</v>
       </c>
       <c r="B1063" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1063" t="n">
         <v>13</v>
@@ -78416,7 +78416,7 @@
         <v>6845</v>
       </c>
       <c r="B1069" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1069" t="n">
         <v>1</v>
@@ -79000,7 +79000,7 @@
         <v>6800</v>
       </c>
       <c r="B1077" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1077" t="n">
         <v>28</v>
@@ -79219,7 +79219,7 @@
         <v>1262</v>
       </c>
       <c r="B1080" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1080" t="n">
         <v>1</v>
@@ -80387,7 +80387,7 @@
         <v>4514</v>
       </c>
       <c r="B1096" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1096" t="n">
         <v>40</v>
@@ -80606,7 +80606,7 @@
         <v>5720</v>
       </c>
       <c r="B1099" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1099" t="n">
         <v>1</v>
@@ -81263,7 +81263,7 @@
         <v>5883</v>
       </c>
       <c r="B1108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1108" t="n">
         <v>45</v>
@@ -82285,7 +82285,7 @@
         <v>1732</v>
       </c>
       <c r="B1122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1122" t="n">
         <v>42</v>
@@ -82723,7 +82723,7 @@
         <v>2071</v>
       </c>
       <c r="B1128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1128" t="n">
         <v>19</v>
@@ -83672,7 +83672,7 @@
         <v>725</v>
       </c>
       <c r="B1141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1141" t="n">
         <v>16</v>
@@ -84402,7 +84402,7 @@
         <v>6343</v>
       </c>
       <c r="B1151" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1151" t="n">
         <v>1</v>
@@ -84840,7 +84840,7 @@
         <v>1405</v>
       </c>
       <c r="B1157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1157" t="n">
         <v>18</v>
@@ -85205,7 +85205,7 @@
         <v>1424</v>
       </c>
       <c r="B1162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1162" t="n">
         <v>10</v>
@@ -85424,7 +85424,7 @@
         <v>367</v>
       </c>
       <c r="B1165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1165" t="n">
         <v>34</v>
@@ -86811,7 +86811,7 @@
         <v>2914</v>
       </c>
       <c r="B1184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1184" t="n">
         <v>60</v>
@@ -89366,7 +89366,7 @@
         <v>422</v>
       </c>
       <c r="B1219" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1219" t="n">
         <v>13</v>
@@ -89804,7 +89804,7 @@
         <v>277</v>
       </c>
       <c r="B1225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1225" t="n">
         <v>23</v>
@@ -89950,7 +89950,7 @@
         <v>5588</v>
       </c>
       <c r="B1227" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1227" t="n">
         <v>22</v>
@@ -91264,7 +91264,7 @@
         <v>2828</v>
       </c>
       <c r="B1245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1245" t="n">
         <v>20</v>
@@ -91483,7 +91483,7 @@
         <v>3035</v>
       </c>
       <c r="B1248" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1248" t="n">
         <v>6</v>
@@ -91556,7 +91556,7 @@
         <v>1532</v>
       </c>
       <c r="B1249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1249" t="n">
         <v>2</v>
@@ -93308,7 +93308,7 @@
         <v>5225</v>
       </c>
       <c r="B1273" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1273" t="n">
         <v>20</v>
@@ -95352,7 +95352,7 @@
         <v>2732</v>
       </c>
       <c r="B1301" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1301" t="n">
         <v>5</v>
@@ -95936,7 +95936,7 @@
         <v>1872</v>
       </c>
       <c r="B1309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1309" t="n">
         <v>22</v>
@@ -97031,7 +97031,7 @@
         <v>750</v>
       </c>
       <c r="B1324" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1324" t="n">
         <v>61</v>
@@ -98856,7 +98856,7 @@
         <v>43</v>
       </c>
       <c r="B1349" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1349" t="n">
         <v>7</v>
@@ -99586,7 +99586,7 @@
         <v>5059</v>
       </c>
       <c r="B1359" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1359" t="n">
         <v>1</v>
@@ -99805,7 +99805,7 @@
         <v>2820</v>
       </c>
       <c r="B1362" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1362" t="n">
         <v>1</v>
@@ -100389,7 +100389,7 @@
         <v>5330</v>
       </c>
       <c r="B1370" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1370" t="n">
         <v>16</v>
@@ -100462,7 +100462,7 @@
         <v>5402</v>
       </c>
       <c r="B1371" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1371" t="n">
         <v>1</v>
@@ -101119,7 +101119,7 @@
         <v>1454</v>
       </c>
       <c r="B1380" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1380" t="n">
         <v>9</v>
@@ -102360,7 +102360,7 @@
         <v>6576</v>
       </c>
       <c r="B1397" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1397" t="n">
         <v>55</v>
@@ -102506,7 +102506,7 @@
         <v>3148</v>
       </c>
       <c r="B1399" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1399" t="n">
         <v>1</v>

</xml_diff>